<commit_message>
Optimisation de l'affichage des produits dans la liste d'inventaire en simplifiant la structure des colonnes. Mise à jour des fichiers Excel 'listes_inventaire.xlsx' et 'produits_listes_inventaire.xlsx' pour refléter les modifications apportées.
</commit_message>
<xml_diff>
--- a/data/listes_inventaire.xlsx
+++ b/data/listes_inventaire.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +465,36 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>INV001</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Inventaire du 2025-06-02_1131</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2025-06-02 11:31:22</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>En préparation</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Utilisateur</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Amélioration du traitement des données lors du chargement des listes d'inventaire et des produits, en s'assurant que les colonnes ID, Nom et Référence sont traitées comme des chaînes de caractères. Ajout de filtres pour une meilleure navigation dans l'affichage des produits disponibles. Mise à jour des fichiers Excel 'listes_inventaire.xlsx' et 'produits_listes_inventaire.xlsx' pour refléter les modifications.
</commit_message>
<xml_diff>
--- a/data/listes_inventaire.xlsx
+++ b/data/listes_inventaire.xlsx
@@ -473,12 +473,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Inventaire du 2025-06-02_1131</t>
+          <t>Inventaire du 2025-06-02_1256</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-02 11:31:22</t>
+          <t>2025-06-02 12:56:51</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>

</xml_diff>